<commit_message>
Date handling has been learnt
</commit_message>
<xml_diff>
--- a/hdv_temp.xlsx
+++ b/hdv_temp.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6690" yWindow="-14850" windowWidth="15375" windowHeight="7785" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-3480" yWindow="-16320" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="NIBP" sheetId="1" state="visible" r:id="rId1"/>
@@ -15,7 +15,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="14">
     <font>
       <name val="Calibri"/>
@@ -133,7 +135,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -352,17 +354,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -461,7 +452,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -491,15 +482,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -520,9 +502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
@@ -541,15 +520,189 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
@@ -562,17 +715,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -580,213 +736,42 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="15" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="14" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1184,8 +1169,8 @@
   </sheetPr>
   <dimension ref="A1:K64"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A43" zoomScale="130" zoomScaleNormal="118" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54:G64"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A23" zoomScale="130" zoomScaleNormal="118" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34:J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -1206,17 +1191,17 @@
       <c r="A1" s="13" t="n"/>
       <c r="B1" s="12" t="n"/>
       <c r="C1" s="11" t="n"/>
-      <c r="D1" s="107" t="inlineStr">
+      <c r="D1" s="104" t="inlineStr">
         <is>
           <t>HOJA DE VIDA</t>
         </is>
       </c>
-      <c r="E1" s="108" t="n"/>
-      <c r="F1" s="108" t="n"/>
-      <c r="G1" s="108" t="n"/>
-      <c r="H1" s="108" t="n"/>
-      <c r="I1" s="108" t="n"/>
-      <c r="J1" s="109" t="n"/>
+      <c r="E1" s="105" t="n"/>
+      <c r="F1" s="105" t="n"/>
+      <c r="G1" s="105" t="n"/>
+      <c r="H1" s="105" t="n"/>
+      <c r="I1" s="105" t="n"/>
+      <c r="J1" s="106" t="n"/>
     </row>
     <row r="2" ht="15" customHeight="1" thickBot="1">
       <c r="A2" s="10" t="n"/>
@@ -1226,18 +1211,18 @@
           <t>F-GRCU-052</t>
         </is>
       </c>
-      <c r="E2" s="110" t="inlineStr">
+      <c r="E2" s="107" t="inlineStr">
         <is>
           <t>GESTION DE RECURSOS</t>
         </is>
       </c>
       <c r="H2" s="9" t="n"/>
-      <c r="I2" s="111" t="inlineStr">
+      <c r="I2" s="108" t="inlineStr">
         <is>
           <t>VERSION 2.0</t>
         </is>
       </c>
-      <c r="J2" s="109" t="n"/>
+      <c r="J2" s="106" t="n"/>
     </row>
     <row r="3" ht="38.25" customHeight="1" thickBot="1">
       <c r="A3" s="7" t="n"/>
@@ -1249,18 +1234,18 @@
         </is>
       </c>
       <c r="E3" s="8" t="n"/>
-      <c r="F3" s="112" t="n"/>
-      <c r="G3" s="112" t="n"/>
-      <c r="H3" s="113" t="n"/>
-      <c r="I3" s="111" t="inlineStr">
+      <c r="F3" s="109" t="n"/>
+      <c r="G3" s="109" t="n"/>
+      <c r="H3" s="110" t="n"/>
+      <c r="I3" s="108" t="inlineStr">
         <is>
           <t>PAG. 1 DE 1</t>
         </is>
       </c>
-      <c r="J3" s="109" t="n"/>
+      <c r="J3" s="106" t="n"/>
     </row>
     <row r="4" ht="21.75" customHeight="1">
-      <c r="A4" s="103" t="inlineStr">
+      <c r="A4" s="49" t="inlineStr">
         <is>
           <t>1. UBICACIÓN GEOGRAFICA DEL EQUIPO</t>
         </is>
@@ -1276,712 +1261,722 @@
       <c r="J4" s="12" t="n"/>
     </row>
     <row r="5" ht="20.25" customHeight="1">
-      <c r="A5" s="101" t="inlineStr">
+      <c r="A5" s="34" t="inlineStr">
         <is>
           <t xml:space="preserve">I. UBICACIÓN GEOGRÁFICA </t>
         </is>
       </c>
-      <c r="B5" s="114" t="n"/>
-      <c r="C5" s="114" t="n"/>
-      <c r="D5" s="114" t="n"/>
-      <c r="E5" s="114" t="n"/>
-      <c r="F5" s="114" t="n"/>
-      <c r="G5" s="114" t="n"/>
-      <c r="H5" s="75" t="n"/>
-      <c r="I5" s="115" t="n"/>
-      <c r="J5" s="116" t="n"/>
+      <c r="B5" s="111" t="n"/>
+      <c r="C5" s="111" t="n"/>
+      <c r="D5" s="111" t="n"/>
+      <c r="E5" s="111" t="n"/>
+      <c r="F5" s="111" t="n"/>
+      <c r="G5" s="111" t="n"/>
+      <c r="H5" s="52" t="n"/>
+      <c r="I5" s="112" t="n"/>
+      <c r="J5" s="113" t="n"/>
     </row>
     <row r="6" ht="16.5" customHeight="1">
-      <c r="A6" s="88" t="inlineStr">
+      <c r="A6" s="54" t="inlineStr">
         <is>
           <t>DEPARTAMENTO</t>
         </is>
       </c>
-      <c r="B6" s="117" t="n"/>
-      <c r="C6" s="92" t="inlineStr">
-        <is>
-          <t>prueba</t>
-        </is>
-      </c>
-      <c r="D6" s="114" t="n"/>
-      <c r="E6" s="114" t="n"/>
-      <c r="F6" s="114" t="n"/>
-      <c r="G6" s="117" t="n"/>
-      <c r="H6" s="118" t="n"/>
-      <c r="J6" s="119" t="n"/>
+      <c r="B6" s="114" t="n"/>
+      <c r="C6" s="55" t="inlineStr">
+        <is>
+          <t>sdggd</t>
+        </is>
+      </c>
+      <c r="D6" s="111" t="n"/>
+      <c r="E6" s="111" t="n"/>
+      <c r="F6" s="111" t="n"/>
+      <c r="G6" s="114" t="n"/>
+      <c r="H6" s="115" t="n"/>
+      <c r="J6" s="116" t="n"/>
     </row>
     <row r="7" ht="15" customHeight="1">
-      <c r="A7" s="88" t="inlineStr">
+      <c r="A7" s="54" t="inlineStr">
         <is>
           <t>MUNICIPIO</t>
         </is>
       </c>
-      <c r="B7" s="117" t="n"/>
-      <c r="C7" s="92" t="inlineStr">
-        <is>
-          <t>desde el front</t>
-        </is>
-      </c>
-      <c r="D7" s="114" t="n"/>
-      <c r="E7" s="114" t="n"/>
-      <c r="F7" s="114" t="n"/>
-      <c r="G7" s="117" t="n"/>
-      <c r="H7" s="118" t="n"/>
-      <c r="J7" s="119" t="n"/>
+      <c r="B7" s="114" t="n"/>
+      <c r="C7" s="55" t="inlineStr">
+        <is>
+          <t>sdsdf</t>
+        </is>
+      </c>
+      <c r="D7" s="111" t="n"/>
+      <c r="E7" s="111" t="n"/>
+      <c r="F7" s="111" t="n"/>
+      <c r="G7" s="114" t="n"/>
+      <c r="H7" s="115" t="n"/>
+      <c r="J7" s="116" t="n"/>
     </row>
     <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="88" t="inlineStr">
+      <c r="A8" s="54" t="inlineStr">
         <is>
           <t>ENTIDAD</t>
         </is>
       </c>
-      <c r="B8" s="117" t="n"/>
-      <c r="C8" s="92" t="inlineStr">
-        <is>
-          <t>Next JS</t>
-        </is>
-      </c>
-      <c r="D8" s="114" t="n"/>
-      <c r="E8" s="114" t="n"/>
-      <c r="F8" s="114" t="n"/>
-      <c r="G8" s="117" t="n"/>
-      <c r="H8" s="118" t="n"/>
-      <c r="J8" s="119" t="n"/>
+      <c r="B8" s="114" t="n"/>
+      <c r="C8" s="55" t="inlineStr">
+        <is>
+          <t>sdff</t>
+        </is>
+      </c>
+      <c r="D8" s="111" t="n"/>
+      <c r="E8" s="111" t="n"/>
+      <c r="F8" s="111" t="n"/>
+      <c r="G8" s="114" t="n"/>
+      <c r="H8" s="115" t="n"/>
+      <c r="J8" s="116" t="n"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="88" t="inlineStr">
+      <c r="A9" s="54" t="inlineStr">
         <is>
           <t xml:space="preserve">CORREO </t>
         </is>
       </c>
-      <c r="B9" s="117" t="n"/>
-      <c r="C9" s="94" t="inlineStr">
-        <is>
-          <t>elcastritupapa@gmail.com</t>
-        </is>
-      </c>
-      <c r="D9" s="114" t="n"/>
-      <c r="E9" s="114" t="n"/>
-      <c r="F9" s="114" t="n"/>
-      <c r="G9" s="117" t="n"/>
-      <c r="H9" s="118" t="n"/>
-      <c r="J9" s="119" t="n"/>
+      <c r="B9" s="114" t="n"/>
+      <c r="C9" s="57" t="inlineStr">
+        <is>
+          <t>sdg</t>
+        </is>
+      </c>
+      <c r="D9" s="111" t="n"/>
+      <c r="E9" s="111" t="n"/>
+      <c r="F9" s="111" t="n"/>
+      <c r="G9" s="114" t="n"/>
+      <c r="H9" s="115" t="n"/>
+      <c r="J9" s="116" t="n"/>
     </row>
     <row r="10">
-      <c r="A10" s="88" t="inlineStr">
+      <c r="A10" s="54" t="inlineStr">
         <is>
           <t>DIRECCIÓN</t>
         </is>
       </c>
-      <c r="B10" s="117" t="n"/>
-      <c r="C10" s="95" t="inlineStr">
-        <is>
-          <t>el rancho de yan</t>
-        </is>
-      </c>
-      <c r="D10" s="114" t="n"/>
-      <c r="E10" s="114" t="n"/>
-      <c r="F10" s="114" t="n"/>
-      <c r="G10" s="117" t="n"/>
-      <c r="H10" s="118" t="n"/>
-      <c r="J10" s="119" t="n"/>
+      <c r="B10" s="114" t="n"/>
+      <c r="C10" s="58" t="inlineStr">
+        <is>
+          <t>fddh</t>
+        </is>
+      </c>
+      <c r="D10" s="111" t="n"/>
+      <c r="E10" s="111" t="n"/>
+      <c r="F10" s="111" t="n"/>
+      <c r="G10" s="114" t="n"/>
+      <c r="H10" s="115" t="n"/>
+      <c r="J10" s="116" t="n"/>
     </row>
     <row r="11" ht="15" customHeight="1">
-      <c r="A11" s="88" t="inlineStr">
+      <c r="A11" s="54" t="inlineStr">
         <is>
           <t>TELÉFONO (S)</t>
         </is>
       </c>
-      <c r="B11" s="117" t="n"/>
-      <c r="C11" s="98" t="inlineStr">
-        <is>
-          <t>3333333</t>
-        </is>
-      </c>
-      <c r="D11" s="114" t="n"/>
-      <c r="E11" s="114" t="n"/>
-      <c r="F11" s="114" t="n"/>
-      <c r="G11" s="117" t="n"/>
-      <c r="H11" s="120" t="n"/>
-      <c r="I11" s="121" t="n"/>
-      <c r="J11" s="122" t="n"/>
+      <c r="B11" s="114" t="n"/>
+      <c r="C11" s="61" t="inlineStr">
+        <is>
+          <t>fghrt</t>
+        </is>
+      </c>
+      <c r="D11" s="111" t="n"/>
+      <c r="E11" s="111" t="n"/>
+      <c r="F11" s="111" t="n"/>
+      <c r="G11" s="114" t="n"/>
+      <c r="H11" s="117" t="n"/>
+      <c r="I11" s="118" t="n"/>
+      <c r="J11" s="119" t="n"/>
     </row>
     <row r="12" ht="24.75" customHeight="1">
-      <c r="A12" s="69" t="inlineStr">
+      <c r="A12" s="31" t="inlineStr">
         <is>
           <t>II. INFORMACIÓN GENERAL</t>
         </is>
       </c>
-      <c r="B12" s="114" t="n"/>
-      <c r="C12" s="114" t="n"/>
-      <c r="D12" s="114" t="n"/>
-      <c r="E12" s="65" t="inlineStr">
+      <c r="B12" s="111" t="n"/>
+      <c r="C12" s="111" t="n"/>
+      <c r="D12" s="111" t="n"/>
+      <c r="E12" s="86" t="inlineStr">
         <is>
           <t>III. REGISTRO HISTORICO</t>
         </is>
       </c>
-      <c r="F12" s="114" t="n"/>
-      <c r="G12" s="114" t="n"/>
-      <c r="H12" s="114" t="n"/>
-      <c r="I12" s="114" t="n"/>
-      <c r="J12" s="117" t="n"/>
+      <c r="F12" s="111" t="n"/>
+      <c r="G12" s="111" t="n"/>
+      <c r="H12" s="111" t="n"/>
+      <c r="I12" s="111" t="n"/>
+      <c r="J12" s="114" t="n"/>
     </row>
     <row r="13" ht="19.5" customHeight="1">
-      <c r="A13" s="76" t="inlineStr">
+      <c r="A13" s="64" t="inlineStr">
         <is>
           <t>EQUIPO:</t>
         </is>
       </c>
-      <c r="B13" s="117" t="n"/>
-      <c r="C13" s="49" t="n"/>
-      <c r="D13" s="114" t="n"/>
-      <c r="E13" s="89" t="inlineStr">
-        <is>
-          <t xml:space="preserve">FORMA DE ADQUISICIÓN:  1. Compra                   2. Donación           3.Incautación                              </t>
-        </is>
-      </c>
-      <c r="F13" s="73" t="n"/>
-      <c r="G13" s="73" t="n"/>
-      <c r="H13" s="73" t="n"/>
-      <c r="I13" s="73" t="n"/>
-      <c r="J13" s="33" t="n"/>
-      <c r="K13" s="32" t="n"/>
+      <c r="B13" s="114" t="n"/>
+      <c r="C13" s="36" t="inlineStr">
+        <is>
+          <t>asdg</t>
+        </is>
+      </c>
+      <c r="D13" s="111" t="n"/>
+      <c r="E13" s="103" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FORMA DE ADQUISICIÓN: </t>
+        </is>
+      </c>
+      <c r="F13" s="111" t="n"/>
+      <c r="G13" s="98" t="n"/>
+      <c r="H13" s="111" t="n"/>
+      <c r="I13" s="111" t="n"/>
+      <c r="J13" s="114" t="n"/>
+      <c r="K13" s="28" t="n"/>
     </row>
     <row r="14" ht="17.25" customHeight="1">
-      <c r="A14" s="76" t="inlineStr">
+      <c r="A14" s="64" t="inlineStr">
         <is>
           <t>MARCA:</t>
         </is>
       </c>
-      <c r="B14" s="117" t="n"/>
-      <c r="C14" s="75" t="n"/>
-      <c r="D14" s="117" t="n"/>
-      <c r="E14" s="123" t="inlineStr">
+      <c r="B14" s="114" t="n"/>
+      <c r="C14" s="52" t="inlineStr">
+        <is>
+          <t>wegrh</t>
+        </is>
+      </c>
+      <c r="D14" s="114" t="n"/>
+      <c r="E14" s="120" t="inlineStr">
         <is>
           <t xml:space="preserve">DOCUMENTO: </t>
         </is>
       </c>
-      <c r="F14" s="114" t="n"/>
-      <c r="G14" s="117" t="n"/>
-      <c r="H14" s="123" t="inlineStr">
+      <c r="F14" s="111" t="n"/>
+      <c r="G14" s="114" t="n"/>
+      <c r="H14" s="120" t="inlineStr">
         <is>
           <t>FACTURA</t>
         </is>
       </c>
-      <c r="I14" s="114" t="n"/>
-      <c r="J14" s="117" t="n"/>
+      <c r="I14" s="111" t="n"/>
+      <c r="J14" s="114" t="n"/>
     </row>
     <row r="15" ht="16.5" customHeight="1">
-      <c r="A15" s="76" t="inlineStr">
+      <c r="A15" s="64" t="inlineStr">
         <is>
           <t>MODELO:</t>
         </is>
       </c>
-      <c r="B15" s="117" t="n"/>
-      <c r="C15" s="75" t="n"/>
-      <c r="D15" s="117" t="n"/>
-      <c r="E15" s="77" t="inlineStr">
+      <c r="B15" s="114" t="n"/>
+      <c r="C15" s="52" t="inlineStr">
+        <is>
+          <t>sdsd</t>
+        </is>
+      </c>
+      <c r="D15" s="114" t="n"/>
+      <c r="E15" s="81" t="inlineStr">
         <is>
           <t xml:space="preserve">AÑO DE FABRICACIÓN:          </t>
         </is>
       </c>
-      <c r="F15" s="117" t="n"/>
-      <c r="G15" s="34" t="n"/>
-      <c r="H15" s="31" t="inlineStr">
+      <c r="F15" s="114" t="n"/>
+      <c r="G15" s="29" t="n"/>
+      <c r="H15" s="27" t="inlineStr">
         <is>
           <t>DIA</t>
         </is>
       </c>
-      <c r="I15" s="31" t="inlineStr">
+      <c r="I15" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">MES </t>
         </is>
       </c>
-      <c r="J15" s="31" t="inlineStr">
+      <c r="J15" s="27" t="inlineStr">
         <is>
           <t>AÑO</t>
         </is>
       </c>
     </row>
     <row r="16" ht="15" customHeight="1">
-      <c r="A16" s="76" t="inlineStr">
+      <c r="A16" s="64" t="inlineStr">
         <is>
           <t>SERIE N°:</t>
         </is>
       </c>
-      <c r="B16" s="117" t="n"/>
-      <c r="C16" s="75" t="n"/>
-      <c r="D16" s="117" t="n"/>
-      <c r="E16" s="88" t="inlineStr">
+      <c r="B16" s="114" t="n"/>
+      <c r="C16" s="52" t="inlineStr">
+        <is>
+          <t>ewer</t>
+        </is>
+      </c>
+      <c r="D16" s="114" t="n"/>
+      <c r="E16" s="54" t="inlineStr">
         <is>
           <t>FECHA DE COMPRA</t>
         </is>
       </c>
-      <c r="F16" s="117" t="n"/>
-      <c r="G16" s="88" t="n"/>
-      <c r="H16" s="92" t="n"/>
-      <c r="I16" s="92" t="n"/>
-      <c r="J16" s="92" t="n"/>
+      <c r="F16" s="114" t="n"/>
+      <c r="G16" s="54" t="n"/>
+      <c r="H16" s="121" t="n">
+        <v>45146</v>
+      </c>
+      <c r="I16" s="55" t="n"/>
+      <c r="J16" s="55" t="n"/>
     </row>
     <row r="17">
-      <c r="A17" s="76" t="inlineStr">
+      <c r="A17" s="64" t="inlineStr">
         <is>
           <t>ACTIVO FIJO:</t>
         </is>
       </c>
-      <c r="B17" s="117" t="n"/>
-      <c r="C17" s="75" t="n"/>
-      <c r="D17" s="117" t="n"/>
-      <c r="E17" s="88" t="inlineStr">
+      <c r="B17" s="114" t="n"/>
+      <c r="C17" s="52" t="inlineStr">
+        <is>
+          <t>wewe</t>
+        </is>
+      </c>
+      <c r="D17" s="114" t="n"/>
+      <c r="E17" s="54" t="inlineStr">
         <is>
           <t>FECHA INSTALACIÓN</t>
         </is>
       </c>
-      <c r="F17" s="114" t="n"/>
-      <c r="G17" s="117" t="n"/>
-      <c r="H17" s="92" t="n"/>
-      <c r="I17" s="92" t="n"/>
-      <c r="J17" s="92" t="n"/>
+      <c r="F17" s="111" t="n"/>
+      <c r="G17" s="114" t="n"/>
+      <c r="H17" s="55" t="n"/>
+      <c r="I17" s="55" t="n"/>
+      <c r="J17" s="55" t="n"/>
     </row>
     <row r="18" ht="15" customHeight="1">
-      <c r="A18" s="76" t="inlineStr">
+      <c r="A18" s="64" t="inlineStr">
         <is>
           <t>REGISTRO SANITARIO:</t>
         </is>
       </c>
-      <c r="B18" s="117" t="n"/>
-      <c r="C18" s="75" t="n"/>
-      <c r="D18" s="117" t="n"/>
-      <c r="E18" s="30" t="inlineStr">
+      <c r="B18" s="114" t="n"/>
+      <c r="C18" s="52" t="inlineStr">
+        <is>
+          <t>asr</t>
+        </is>
+      </c>
+      <c r="D18" s="114" t="n"/>
+      <c r="E18" s="26" t="inlineStr">
         <is>
           <t>INICIO DE OPERACIÓN</t>
         </is>
       </c>
-      <c r="F18" s="30" t="n"/>
-      <c r="G18" s="30" t="n"/>
-      <c r="H18" s="92" t="n"/>
-      <c r="I18" s="92" t="n"/>
-      <c r="J18" s="92" t="n"/>
+      <c r="F18" s="26" t="n"/>
+      <c r="G18" s="26" t="n"/>
+      <c r="H18" s="55" t="n"/>
+      <c r="I18" s="55" t="n"/>
+      <c r="J18" s="55" t="n"/>
     </row>
     <row r="19" ht="15" customHeight="1">
-      <c r="A19" s="76" t="inlineStr">
+      <c r="A19" s="64" t="inlineStr">
         <is>
           <t>UBICACIÓN:</t>
         </is>
       </c>
-      <c r="B19" s="117" t="n"/>
-      <c r="C19" s="124" t="n"/>
-      <c r="D19" s="117" t="n"/>
-      <c r="E19" s="88" t="inlineStr">
+      <c r="B19" s="114" t="n"/>
+      <c r="C19" s="122" t="inlineStr">
+        <is>
+          <t>ewter</t>
+        </is>
+      </c>
+      <c r="D19" s="114" t="n"/>
+      <c r="E19" s="54" t="inlineStr">
         <is>
           <t>VENCIMIENTO DE GARANTIA</t>
         </is>
       </c>
-      <c r="F19" s="114" t="n"/>
-      <c r="G19" s="117" t="n"/>
-      <c r="H19" s="92" t="n"/>
-      <c r="I19" s="92" t="n"/>
-      <c r="J19" s="92" t="n"/>
+      <c r="F19" s="111" t="n"/>
+      <c r="G19" s="114" t="n"/>
+      <c r="H19" s="55" t="n"/>
+      <c r="I19" s="55" t="n"/>
+      <c r="J19" s="55" t="n"/>
     </row>
     <row r="20" ht="15" customHeight="1">
-      <c r="A20" s="27" t="inlineStr">
+      <c r="A20" s="23" t="inlineStr">
         <is>
           <t>PROVEEDOR:</t>
         </is>
       </c>
-      <c r="B20" s="26" t="n"/>
-      <c r="C20" s="75" t="n"/>
-      <c r="D20" s="117" t="n"/>
-      <c r="E20" s="125" t="inlineStr">
+      <c r="B20" s="22" t="n"/>
+      <c r="C20" s="52" t="inlineStr">
+        <is>
+          <t>erer</t>
+        </is>
+      </c>
+      <c r="D20" s="114" t="n"/>
+      <c r="E20" s="123" t="inlineStr">
         <is>
           <t>FABRICANTE: CHINA.</t>
         </is>
       </c>
-      <c r="F20" s="114" t="n"/>
-      <c r="G20" s="117" t="n"/>
-      <c r="H20" s="35" t="inlineStr">
+      <c r="F20" s="111" t="n"/>
+      <c r="G20" s="114" t="n"/>
+      <c r="H20" s="30" t="inlineStr">
         <is>
           <t>NOMBRE:</t>
         </is>
       </c>
-      <c r="I20" s="45" t="n"/>
-      <c r="J20" s="117" t="n"/>
+      <c r="I20" s="100" t="n"/>
+      <c r="J20" s="114" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="24" t="n"/>
-      <c r="B21" s="23" t="n"/>
-      <c r="C21" s="23" t="n"/>
-      <c r="D21" s="23" t="n"/>
-      <c r="E21" s="23" t="n"/>
-      <c r="F21" s="23" t="n"/>
-      <c r="G21" s="23" t="n"/>
-      <c r="H21" s="23" t="n"/>
-      <c r="I21" s="23" t="n"/>
-      <c r="J21" s="22" t="n"/>
+      <c r="A21" s="21" t="n"/>
+      <c r="B21" s="20" t="n"/>
+      <c r="C21" s="20" t="n"/>
+      <c r="D21" s="20" t="n"/>
+      <c r="E21" s="20" t="n"/>
+      <c r="F21" s="20" t="n"/>
+      <c r="G21" s="20" t="n"/>
+      <c r="H21" s="20" t="n"/>
+      <c r="I21" s="20" t="n"/>
+      <c r="J21" s="19" t="n"/>
     </row>
     <row r="22" ht="25.5" customHeight="1">
-      <c r="A22" s="126" t="inlineStr">
+      <c r="A22" s="124" t="inlineStr">
         <is>
           <t xml:space="preserve">              IV. REGISTRO TÉCNICO DE INSTALACIÓN</t>
         </is>
       </c>
-      <c r="B22" s="114" t="n"/>
-      <c r="C22" s="114" t="n"/>
-      <c r="D22" s="114" t="n"/>
-      <c r="E22" s="114" t="n"/>
-      <c r="F22" s="114" t="n"/>
-      <c r="G22" s="114" t="n"/>
-      <c r="H22" s="114" t="n"/>
-      <c r="I22" s="114" t="n"/>
-      <c r="J22" s="117" t="n"/>
+      <c r="B22" s="111" t="n"/>
+      <c r="C22" s="111" t="n"/>
+      <c r="D22" s="111" t="n"/>
+      <c r="E22" s="111" t="n"/>
+      <c r="F22" s="111" t="n"/>
+      <c r="G22" s="111" t="n"/>
+      <c r="H22" s="111" t="n"/>
+      <c r="I22" s="111" t="n"/>
+      <c r="J22" s="114" t="n"/>
     </row>
     <row r="23">
-      <c r="A23" s="79" t="inlineStr">
+      <c r="A23" s="77" t="inlineStr">
         <is>
           <t>TENSIÓN (V)</t>
         </is>
       </c>
-      <c r="B23" s="117" t="n"/>
-      <c r="C23" s="80" t="n"/>
-      <c r="D23" s="117" t="n"/>
-      <c r="E23" s="76" t="inlineStr">
+      <c r="B23" s="114" t="n"/>
+      <c r="C23" s="78" t="n"/>
+      <c r="D23" s="114" t="n"/>
+      <c r="E23" s="64" t="inlineStr">
         <is>
           <t xml:space="preserve">CORRIENTE (A):  </t>
         </is>
       </c>
-      <c r="F23" s="117" t="n"/>
-      <c r="G23" s="21" t="n"/>
-      <c r="H23" s="98" t="inlineStr">
+      <c r="F23" s="114" t="n"/>
+      <c r="G23" s="18" t="n"/>
+      <c r="H23" s="61" t="inlineStr">
         <is>
           <t xml:space="preserve">PESO: </t>
         </is>
       </c>
-      <c r="I23" s="117" t="n"/>
-      <c r="J23" s="20" t="n"/>
+      <c r="I23" s="114" t="n"/>
+      <c r="J23" s="17" t="n"/>
     </row>
     <row r="24">
-      <c r="A24" s="79" t="inlineStr">
+      <c r="A24" s="77" t="inlineStr">
         <is>
           <t>POTENCIA (W)</t>
         </is>
       </c>
-      <c r="B24" s="117" t="n"/>
-      <c r="C24" s="80" t="n"/>
-      <c r="D24" s="117" t="n"/>
-      <c r="E24" s="76" t="inlineStr">
+      <c r="B24" s="114" t="n"/>
+      <c r="C24" s="78" t="n"/>
+      <c r="D24" s="114" t="n"/>
+      <c r="E24" s="64" t="inlineStr">
         <is>
           <t>FRECUENCIA (Hz):</t>
         </is>
       </c>
-      <c r="F24" s="117" t="n"/>
-      <c r="G24" s="21" t="n"/>
-      <c r="H24" s="98" t="inlineStr">
+      <c r="F24" s="114" t="n"/>
+      <c r="G24" s="18" t="n"/>
+      <c r="H24" s="61" t="inlineStr">
         <is>
           <t>VELOCIDAD:</t>
         </is>
       </c>
-      <c r="I24" s="117" t="n"/>
-      <c r="J24" s="20" t="n"/>
+      <c r="I24" s="114" t="n"/>
+      <c r="J24" s="17" t="n"/>
     </row>
     <row r="25" ht="16.5" customHeight="1">
-      <c r="A25" s="79" t="inlineStr">
+      <c r="A25" s="77" t="inlineStr">
         <is>
           <t>PRESION</t>
         </is>
       </c>
-      <c r="B25" s="117" t="n"/>
-      <c r="C25" s="80" t="n"/>
-      <c r="D25" s="117" t="n"/>
-      <c r="E25" s="127" t="inlineStr">
+      <c r="B25" s="114" t="n"/>
+      <c r="C25" s="78" t="n"/>
+      <c r="D25" s="114" t="n"/>
+      <c r="E25" s="125" t="inlineStr">
         <is>
           <t>RANGO DE TEMPERATURA</t>
         </is>
       </c>
-      <c r="F25" s="117" t="n"/>
-      <c r="G25" s="19" t="n"/>
-      <c r="H25" s="128" t="inlineStr">
+      <c r="F25" s="114" t="n"/>
+      <c r="G25" s="16" t="n"/>
+      <c r="H25" s="126" t="inlineStr">
         <is>
           <t>TECNOLOGIA PREDOMINANTE</t>
         </is>
       </c>
-      <c r="I25" s="117" t="n"/>
-      <c r="J25" s="18" t="n"/>
+      <c r="I25" s="114" t="n"/>
+      <c r="J25" s="15" t="n"/>
     </row>
     <row r="26" ht="21" customHeight="1">
-      <c r="A26" s="65" t="inlineStr">
+      <c r="A26" s="86" t="inlineStr">
         <is>
           <t>V. REGISTRO TECNICO DE FUNCIONAMIENTO</t>
         </is>
       </c>
-      <c r="B26" s="114" t="n"/>
-      <c r="C26" s="114" t="n"/>
-      <c r="D26" s="117" t="n"/>
-      <c r="E26" s="65" t="inlineStr">
+      <c r="B26" s="111" t="n"/>
+      <c r="C26" s="111" t="n"/>
+      <c r="D26" s="114" t="n"/>
+      <c r="E26" s="86" t="inlineStr">
         <is>
           <t>VI. CLASIFICACIÓN BIOMEDICA</t>
         </is>
       </c>
-      <c r="F26" s="114" t="n"/>
-      <c r="G26" s="114" t="n"/>
-      <c r="H26" s="114" t="n"/>
-      <c r="I26" s="114" t="n"/>
-      <c r="J26" s="117" t="n"/>
+      <c r="F26" s="111" t="n"/>
+      <c r="G26" s="111" t="n"/>
+      <c r="H26" s="111" t="n"/>
+      <c r="I26" s="111" t="n"/>
+      <c r="J26" s="114" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="76" t="inlineStr">
+      <c r="A27" s="64" t="inlineStr">
         <is>
           <t>RANGO DE VOLTAJE:</t>
         </is>
       </c>
-      <c r="B27" s="117" t="n"/>
-      <c r="C27" s="77" t="n"/>
-      <c r="D27" s="117" t="n"/>
-      <c r="E27" s="78" t="inlineStr">
+      <c r="B27" s="114" t="n"/>
+      <c r="C27" s="81" t="n"/>
+      <c r="D27" s="114" t="n"/>
+      <c r="E27" s="82" t="inlineStr">
         <is>
           <t>DIAGNOSTICO</t>
         </is>
       </c>
-      <c r="F27" s="114" t="n"/>
-      <c r="G27" s="117" t="n"/>
-      <c r="H27" s="77" t="n"/>
-      <c r="I27" s="114" t="n"/>
-      <c r="J27" s="117" t="n"/>
+      <c r="F27" s="111" t="n"/>
+      <c r="G27" s="114" t="n"/>
+      <c r="H27" s="81" t="n"/>
+      <c r="I27" s="111" t="n"/>
+      <c r="J27" s="114" t="n"/>
     </row>
     <row r="28">
-      <c r="A28" s="76" t="inlineStr">
+      <c r="A28" s="64" t="inlineStr">
         <is>
           <t>RANGO DE PRESIÓN:</t>
         </is>
       </c>
-      <c r="B28" s="117" t="n"/>
-      <c r="C28" s="77" t="n"/>
-      <c r="D28" s="117" t="n"/>
-      <c r="E28" s="78" t="inlineStr">
+      <c r="B28" s="114" t="n"/>
+      <c r="C28" s="81" t="n"/>
+      <c r="D28" s="114" t="n"/>
+      <c r="E28" s="82" t="inlineStr">
         <is>
           <t>REHABILITACIÓN</t>
         </is>
       </c>
-      <c r="F28" s="114" t="n"/>
-      <c r="G28" s="117" t="n"/>
-      <c r="H28" s="77" t="n"/>
-      <c r="I28" s="114" t="n"/>
-      <c r="J28" s="117" t="n"/>
+      <c r="F28" s="111" t="n"/>
+      <c r="G28" s="114" t="n"/>
+      <c r="H28" s="81" t="n"/>
+      <c r="I28" s="111" t="n"/>
+      <c r="J28" s="114" t="n"/>
     </row>
     <row r="29">
-      <c r="A29" s="76" t="inlineStr">
+      <c r="A29" s="64" t="inlineStr">
         <is>
           <t>RANGO DE HUMEDAD:</t>
         </is>
       </c>
-      <c r="B29" s="117" t="n"/>
-      <c r="C29" s="77" t="n"/>
-      <c r="D29" s="117" t="n"/>
-      <c r="E29" s="78" t="inlineStr">
+      <c r="B29" s="114" t="n"/>
+      <c r="C29" s="81" t="n"/>
+      <c r="D29" s="114" t="n"/>
+      <c r="E29" s="82" t="inlineStr">
         <is>
           <t>PREVENCIÓN</t>
         </is>
       </c>
-      <c r="F29" s="114" t="n"/>
-      <c r="G29" s="117" t="n"/>
-      <c r="H29" s="77" t="n"/>
-      <c r="I29" s="114" t="n"/>
-      <c r="J29" s="117" t="n"/>
+      <c r="F29" s="111" t="n"/>
+      <c r="G29" s="114" t="n"/>
+      <c r="H29" s="81" t="n"/>
+      <c r="I29" s="111" t="n"/>
+      <c r="J29" s="114" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="76" t="inlineStr">
+      <c r="A30" s="64" t="inlineStr">
         <is>
           <t>RANGO DE CORRIENTE:</t>
         </is>
       </c>
-      <c r="B30" s="117" t="n"/>
-      <c r="C30" s="77" t="n"/>
-      <c r="D30" s="117" t="n"/>
-      <c r="E30" s="78" t="inlineStr">
+      <c r="B30" s="114" t="n"/>
+      <c r="C30" s="81" t="n"/>
+      <c r="D30" s="114" t="n"/>
+      <c r="E30" s="82" t="inlineStr">
         <is>
           <t>TRATAMIENTO Y/O MNTO. DE VIDA</t>
         </is>
       </c>
-      <c r="F30" s="114" t="n"/>
-      <c r="G30" s="117" t="n"/>
-      <c r="H30" s="77" t="n"/>
-      <c r="I30" s="114" t="n"/>
-      <c r="J30" s="117" t="n"/>
+      <c r="F30" s="111" t="n"/>
+      <c r="G30" s="114" t="n"/>
+      <c r="H30" s="81" t="n"/>
+      <c r="I30" s="111" t="n"/>
+      <c r="J30" s="114" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="76" t="inlineStr">
+      <c r="A31" s="64" t="inlineStr">
         <is>
           <t>RANGO DE FRECUENCIA:</t>
         </is>
       </c>
-      <c r="B31" s="117" t="n"/>
-      <c r="C31" s="77" t="n"/>
-      <c r="D31" s="117" t="n"/>
-      <c r="E31" s="78" t="inlineStr">
+      <c r="B31" s="114" t="n"/>
+      <c r="C31" s="81" t="n"/>
+      <c r="D31" s="114" t="n"/>
+      <c r="E31" s="82" t="inlineStr">
         <is>
           <t>ANÁLISIS DE LABORATORIO</t>
         </is>
       </c>
-      <c r="F31" s="114" t="n"/>
-      <c r="G31" s="117" t="n"/>
-      <c r="H31" s="77" t="n"/>
-      <c r="I31" s="114" t="n"/>
-      <c r="J31" s="117" t="n"/>
+      <c r="F31" s="111" t="n"/>
+      <c r="G31" s="114" t="n"/>
+      <c r="H31" s="81" t="n"/>
+      <c r="I31" s="111" t="n"/>
+      <c r="J31" s="114" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="77" t="n"/>
-      <c r="B32" s="114" t="n"/>
-      <c r="C32" s="114" t="n"/>
-      <c r="D32" s="114" t="n"/>
-      <c r="E32" s="114" t="n"/>
-      <c r="F32" s="114" t="n"/>
-      <c r="G32" s="114" t="n"/>
-      <c r="H32" s="114" t="n"/>
-      <c r="I32" s="114" t="n"/>
-      <c r="J32" s="117" t="n"/>
+      <c r="A32" s="81" t="n"/>
+      <c r="B32" s="111" t="n"/>
+      <c r="C32" s="111" t="n"/>
+      <c r="D32" s="111" t="n"/>
+      <c r="E32" s="111" t="n"/>
+      <c r="F32" s="111" t="n"/>
+      <c r="G32" s="111" t="n"/>
+      <c r="H32" s="111" t="n"/>
+      <c r="I32" s="111" t="n"/>
+      <c r="J32" s="114" t="n"/>
     </row>
     <row r="33" ht="26.25" customHeight="1">
-      <c r="A33" s="65" t="inlineStr">
+      <c r="A33" s="86" t="inlineStr">
         <is>
           <t>VII. CLASIFICACIÓN SEGÚN NIVEL DE RIESGO</t>
         </is>
       </c>
-      <c r="B33" s="114" t="n"/>
-      <c r="C33" s="114" t="n"/>
-      <c r="D33" s="117" t="n"/>
-      <c r="E33" s="126" t="inlineStr">
+      <c r="B33" s="111" t="n"/>
+      <c r="C33" s="111" t="n"/>
+      <c r="D33" s="114" t="n"/>
+      <c r="E33" s="124" t="inlineStr">
         <is>
           <t>IIX. PERIODICIDAD DEL MANTENIMIENTO:</t>
         </is>
       </c>
-      <c r="F33" s="114" t="n"/>
-      <c r="G33" s="117" t="n"/>
-      <c r="H33" s="65" t="inlineStr">
+      <c r="F33" s="111" t="n"/>
+      <c r="G33" s="114" t="n"/>
+      <c r="H33" s="86" t="inlineStr">
         <is>
           <t>IX. REQUIERE CALIBRACIÓN</t>
         </is>
       </c>
-      <c r="I33" s="114" t="n"/>
-      <c r="J33" s="117" t="n"/>
+      <c r="I33" s="111" t="n"/>
+      <c r="J33" s="114" t="n"/>
     </row>
     <row r="34" ht="17.25" customHeight="1">
-      <c r="A34" s="76" t="inlineStr">
+      <c r="A34" s="82" t="inlineStr">
         <is>
           <t>CLASE I</t>
         </is>
       </c>
-      <c r="B34" s="76" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CLASE IA </t>
-        </is>
-      </c>
-      <c r="C34" s="76" t="inlineStr">
-        <is>
-          <t xml:space="preserve">CLASE IIB  </t>
-        </is>
-      </c>
-      <c r="D34" s="76" t="inlineStr">
-        <is>
-          <t>CLASE III</t>
-        </is>
-      </c>
-      <c r="E34" s="78" t="inlineStr">
+      <c r="B34" s="111" t="n"/>
+      <c r="C34" s="111" t="n"/>
+      <c r="D34" s="114" t="n"/>
+      <c r="E34" s="82" t="inlineStr">
         <is>
           <t>CADA TRES MESES</t>
         </is>
       </c>
-      <c r="F34" s="114" t="n"/>
-      <c r="G34" s="117" t="n"/>
-      <c r="H34" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">SI </t>
-        </is>
-      </c>
-      <c r="I34" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">NO  </t>
-        </is>
-      </c>
-      <c r="J34" s="15" t="inlineStr">
-        <is>
-          <t xml:space="preserve">ANUAL    </t>
-        </is>
-      </c>
+      <c r="F34" s="111" t="n"/>
+      <c r="G34" s="114" t="n"/>
+      <c r="H34" s="82" t="n"/>
+      <c r="I34" s="111" t="n"/>
+      <c r="J34" s="114" t="n"/>
     </row>
     <row r="35" ht="22.5" customHeight="1">
-      <c r="A35" s="65" t="inlineStr">
+      <c r="A35" s="86" t="inlineStr">
         <is>
           <t>X. ACCESORIOS</t>
         </is>
       </c>
-      <c r="B35" s="114" t="n"/>
-      <c r="C35" s="114" t="n"/>
-      <c r="D35" s="114" t="n"/>
-      <c r="E35" s="114" t="n"/>
-      <c r="F35" s="114" t="n"/>
-      <c r="G35" s="114" t="n"/>
-      <c r="H35" s="114" t="n"/>
-      <c r="I35" s="114" t="n"/>
-      <c r="J35" s="117" t="n"/>
+      <c r="B35" s="111" t="n"/>
+      <c r="C35" s="111" t="n"/>
+      <c r="D35" s="111" t="n"/>
+      <c r="E35" s="111" t="n"/>
+      <c r="F35" s="111" t="n"/>
+      <c r="G35" s="111" t="n"/>
+      <c r="H35" s="111" t="n"/>
+      <c r="I35" s="111" t="n"/>
+      <c r="J35" s="114" t="n"/>
     </row>
     <row r="36" ht="20.25" customHeight="1">
-      <c r="A36" s="75" t="inlineStr">
+      <c r="A36" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">1. </t>
         </is>
       </c>
-      <c r="B36" s="114" t="n"/>
-      <c r="C36" s="114" t="n"/>
-      <c r="D36" s="117" t="n"/>
-      <c r="E36" s="75" t="inlineStr">
+      <c r="B36" s="111" t="n"/>
+      <c r="C36" s="111" t="n"/>
+      <c r="D36" s="114" t="n"/>
+      <c r="E36" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">4. </t>
         </is>
       </c>
-      <c r="F36" s="114" t="n"/>
-      <c r="G36" s="114" t="n"/>
-      <c r="H36" s="114" t="n"/>
-      <c r="I36" s="114" t="n"/>
-      <c r="J36" s="117" t="n"/>
+      <c r="F36" s="111" t="n"/>
+      <c r="G36" s="111" t="n"/>
+      <c r="H36" s="111" t="n"/>
+      <c r="I36" s="111" t="n"/>
+      <c r="J36" s="114" t="n"/>
     </row>
     <row r="37" ht="18.75" customHeight="1">
-      <c r="A37" s="75" t="inlineStr">
+      <c r="A37" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">2. </t>
         </is>
       </c>
-      <c r="B37" s="114" t="n"/>
-      <c r="C37" s="114" t="n"/>
-      <c r="D37" s="117" t="n"/>
-      <c r="E37" s="75" t="inlineStr">
+      <c r="B37" s="111" t="n"/>
+      <c r="C37" s="111" t="n"/>
+      <c r="D37" s="114" t="n"/>
+      <c r="E37" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">5. </t>
         </is>
       </c>
-      <c r="F37" s="114" t="n"/>
-      <c r="G37" s="114" t="n"/>
-      <c r="H37" s="114" t="n"/>
-      <c r="I37" s="114" t="n"/>
-      <c r="J37" s="117" t="n"/>
+      <c r="F37" s="111" t="n"/>
+      <c r="G37" s="111" t="n"/>
+      <c r="H37" s="111" t="n"/>
+      <c r="I37" s="111" t="n"/>
+      <c r="J37" s="114" t="n"/>
     </row>
     <row r="38" ht="17.25" customHeight="1">
-      <c r="A38" s="75" t="inlineStr">
+      <c r="A38" s="52" t="inlineStr">
         <is>
           <t xml:space="preserve">3. </t>
         </is>
       </c>
-      <c r="B38" s="114" t="n"/>
-      <c r="C38" s="114" t="n"/>
-      <c r="D38" s="117" t="n"/>
-      <c r="E38" s="75" t="inlineStr">
+      <c r="B38" s="111" t="n"/>
+      <c r="C38" s="111" t="n"/>
+      <c r="D38" s="114" t="n"/>
+      <c r="E38" s="52" t="inlineStr">
         <is>
           <t>6.</t>
         </is>
       </c>
-      <c r="F38" s="114" t="n"/>
-      <c r="G38" s="114" t="n"/>
-      <c r="H38" s="114" t="n"/>
-      <c r="I38" s="114" t="n"/>
-      <c r="J38" s="117" t="n"/>
+      <c r="F38" s="111" t="n"/>
+      <c r="G38" s="111" t="n"/>
+      <c r="H38" s="111" t="n"/>
+      <c r="I38" s="111" t="n"/>
+      <c r="J38" s="114" t="n"/>
     </row>
     <row r="39" ht="24.75" customHeight="1">
       <c r="A39" s="3" t="inlineStr">
@@ -1989,83 +1984,83 @@
           <t xml:space="preserve">XI.  OBSERVACIONES </t>
         </is>
       </c>
-      <c r="B39" s="114" t="n"/>
-      <c r="C39" s="114" t="n"/>
-      <c r="D39" s="114" t="n"/>
-      <c r="E39" s="114" t="n"/>
-      <c r="F39" s="114" t="n"/>
-      <c r="G39" s="114" t="n"/>
-      <c r="H39" s="114" t="n"/>
-      <c r="I39" s="114" t="n"/>
-      <c r="J39" s="117" t="n"/>
+      <c r="B39" s="111" t="n"/>
+      <c r="C39" s="111" t="n"/>
+      <c r="D39" s="111" t="n"/>
+      <c r="E39" s="111" t="n"/>
+      <c r="F39" s="111" t="n"/>
+      <c r="G39" s="111" t="n"/>
+      <c r="H39" s="111" t="n"/>
+      <c r="I39" s="111" t="n"/>
+      <c r="J39" s="114" t="n"/>
     </row>
     <row r="40">
-      <c r="A40" s="75" t="n"/>
-      <c r="B40" s="114" t="n"/>
-      <c r="C40" s="114" t="n"/>
-      <c r="D40" s="114" t="n"/>
-      <c r="E40" s="114" t="n"/>
-      <c r="F40" s="114" t="n"/>
-      <c r="G40" s="114" t="n"/>
-      <c r="H40" s="114" t="n"/>
-      <c r="I40" s="114" t="n"/>
-      <c r="J40" s="117" t="n"/>
+      <c r="A40" s="52" t="n"/>
+      <c r="B40" s="111" t="n"/>
+      <c r="C40" s="111" t="n"/>
+      <c r="D40" s="111" t="n"/>
+      <c r="E40" s="111" t="n"/>
+      <c r="F40" s="111" t="n"/>
+      <c r="G40" s="111" t="n"/>
+      <c r="H40" s="111" t="n"/>
+      <c r="I40" s="111" t="n"/>
+      <c r="J40" s="114" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="75" t="n"/>
-      <c r="B41" s="114" t="n"/>
-      <c r="C41" s="114" t="n"/>
-      <c r="D41" s="114" t="n"/>
-      <c r="E41" s="114" t="n"/>
-      <c r="F41" s="114" t="n"/>
-      <c r="G41" s="114" t="n"/>
-      <c r="H41" s="114" t="n"/>
-      <c r="I41" s="114" t="n"/>
-      <c r="J41" s="117" t="n"/>
+      <c r="A41" s="52" t="n"/>
+      <c r="B41" s="111" t="n"/>
+      <c r="C41" s="111" t="n"/>
+      <c r="D41" s="111" t="n"/>
+      <c r="E41" s="111" t="n"/>
+      <c r="F41" s="111" t="n"/>
+      <c r="G41" s="111" t="n"/>
+      <c r="H41" s="111" t="n"/>
+      <c r="I41" s="111" t="n"/>
+      <c r="J41" s="114" t="n"/>
     </row>
     <row r="42">
-      <c r="A42" s="75" t="n"/>
-      <c r="B42" s="114" t="n"/>
-      <c r="C42" s="114" t="n"/>
-      <c r="D42" s="114" t="n"/>
-      <c r="E42" s="114" t="n"/>
-      <c r="F42" s="114" t="n"/>
-      <c r="G42" s="114" t="n"/>
-      <c r="H42" s="114" t="n"/>
-      <c r="I42" s="114" t="n"/>
-      <c r="J42" s="117" t="n"/>
+      <c r="A42" s="52" t="n"/>
+      <c r="B42" s="111" t="n"/>
+      <c r="C42" s="111" t="n"/>
+      <c r="D42" s="111" t="n"/>
+      <c r="E42" s="111" t="n"/>
+      <c r="F42" s="111" t="n"/>
+      <c r="G42" s="111" t="n"/>
+      <c r="H42" s="111" t="n"/>
+      <c r="I42" s="111" t="n"/>
+      <c r="J42" s="114" t="n"/>
     </row>
     <row r="43" ht="15" customHeight="1">
-      <c r="A43" s="52" t="inlineStr">
+      <c r="A43" s="101" t="inlineStr">
         <is>
           <t>NR: NO REGISTRA</t>
         </is>
       </c>
-      <c r="B43" s="117" t="n"/>
-      <c r="C43" s="52" t="inlineStr">
+      <c r="B43" s="114" t="n"/>
+      <c r="C43" s="101" t="inlineStr">
         <is>
           <t xml:space="preserve">NT: NO TIENE </t>
         </is>
       </c>
-      <c r="D43" s="117" t="n"/>
-      <c r="E43" s="52" t="inlineStr">
+      <c r="D43" s="114" t="n"/>
+      <c r="E43" s="101" t="inlineStr">
         <is>
           <t>AX: ANEXO</t>
         </is>
       </c>
-      <c r="F43" s="117" t="n"/>
-      <c r="G43" s="52" t="inlineStr">
+      <c r="F43" s="114" t="n"/>
+      <c r="G43" s="101" t="inlineStr">
         <is>
           <t>NAX: NO ANEXO</t>
         </is>
       </c>
-      <c r="H43" s="117" t="n"/>
-      <c r="I43" s="52" t="inlineStr">
+      <c r="H43" s="114" t="n"/>
+      <c r="I43" s="101" t="inlineStr">
         <is>
           <t>NA: NO APLICA</t>
         </is>
       </c>
-      <c r="J43" s="117" t="n"/>
+      <c r="J43" s="114" t="n"/>
     </row>
     <row r="44">
       <c r="A44" s="14" t="n"/>
@@ -2108,17 +2103,17 @@
       <c r="A49" s="13" t="n"/>
       <c r="B49" s="12" t="n"/>
       <c r="C49" s="11" t="n"/>
-      <c r="D49" s="107" t="inlineStr">
+      <c r="D49" s="104" t="inlineStr">
         <is>
           <t>HOJA DE VIDA</t>
         </is>
       </c>
-      <c r="E49" s="108" t="n"/>
-      <c r="F49" s="108" t="n"/>
-      <c r="G49" s="108" t="n"/>
-      <c r="H49" s="108" t="n"/>
-      <c r="I49" s="108" t="n"/>
-      <c r="J49" s="109" t="n"/>
+      <c r="E49" s="105" t="n"/>
+      <c r="F49" s="105" t="n"/>
+      <c r="G49" s="105" t="n"/>
+      <c r="H49" s="105" t="n"/>
+      <c r="I49" s="105" t="n"/>
+      <c r="J49" s="106" t="n"/>
     </row>
     <row r="50" ht="33.75" customHeight="1" thickBot="1">
       <c r="A50" s="10" t="n"/>
@@ -2128,18 +2123,18 @@
           <t>F-GRCU-052</t>
         </is>
       </c>
-      <c r="E50" s="110" t="inlineStr">
+      <c r="E50" s="107" t="inlineStr">
         <is>
           <t>GESTION DE RECURSOS</t>
         </is>
       </c>
       <c r="H50" s="9" t="n"/>
-      <c r="I50" s="111" t="inlineStr">
+      <c r="I50" s="108" t="inlineStr">
         <is>
           <t>VERSION 2.0</t>
         </is>
       </c>
-      <c r="J50" s="109" t="n"/>
+      <c r="J50" s="106" t="n"/>
     </row>
     <row r="51" ht="20.25" customHeight="1" thickBot="1">
       <c r="A51" s="7" t="n"/>
@@ -2151,15 +2146,15 @@
         </is>
       </c>
       <c r="E51" s="8" t="n"/>
-      <c r="F51" s="112" t="n"/>
-      <c r="G51" s="112" t="n"/>
-      <c r="H51" s="113" t="n"/>
-      <c r="I51" s="111" t="inlineStr">
+      <c r="F51" s="109" t="n"/>
+      <c r="G51" s="109" t="n"/>
+      <c r="H51" s="110" t="n"/>
+      <c r="I51" s="108" t="inlineStr">
         <is>
           <t>PAG. 2 DE 2</t>
         </is>
       </c>
-      <c r="J51" s="109" t="n"/>
+      <c r="J51" s="106" t="n"/>
     </row>
     <row r="52">
       <c r="A52" s="3" t="inlineStr">
@@ -2167,24 +2162,24 @@
           <t xml:space="preserve">LISTA DE CHEQUEO DE DOCUMENTOS SOPORTES ANEXOS A LA HOJA DE VIDA </t>
         </is>
       </c>
-      <c r="B52" s="114" t="n"/>
-      <c r="C52" s="114" t="n"/>
-      <c r="D52" s="114" t="n"/>
-      <c r="E52" s="114" t="n"/>
-      <c r="F52" s="114" t="n"/>
-      <c r="G52" s="114" t="n"/>
-      <c r="H52" s="114" t="n"/>
-      <c r="I52" s="114" t="n"/>
-      <c r="J52" s="117" t="n"/>
+      <c r="B52" s="111" t="n"/>
+      <c r="C52" s="111" t="n"/>
+      <c r="D52" s="111" t="n"/>
+      <c r="E52" s="111" t="n"/>
+      <c r="F52" s="111" t="n"/>
+      <c r="G52" s="111" t="n"/>
+      <c r="H52" s="111" t="n"/>
+      <c r="I52" s="111" t="n"/>
+      <c r="J52" s="114" t="n"/>
     </row>
     <row r="53">
       <c r="A53" s="2" t="n"/>
-      <c r="B53" s="114" t="n"/>
-      <c r="C53" s="114" t="n"/>
-      <c r="D53" s="114" t="n"/>
-      <c r="E53" s="114" t="n"/>
-      <c r="F53" s="114" t="n"/>
-      <c r="G53" s="117" t="n"/>
+      <c r="B53" s="111" t="n"/>
+      <c r="C53" s="111" t="n"/>
+      <c r="D53" s="111" t="n"/>
+      <c r="E53" s="111" t="n"/>
+      <c r="F53" s="111" t="n"/>
+      <c r="G53" s="114" t="n"/>
       <c r="H53" s="3" t="inlineStr">
         <is>
           <t>AX</t>
@@ -2207,12 +2202,12 @@
           <t>COPIA REGISTRO SANITARIO O PERMISO DE COMERCIALIZACIÓN</t>
         </is>
       </c>
-      <c r="B54" s="114" t="n"/>
-      <c r="C54" s="114" t="n"/>
-      <c r="D54" s="114" t="n"/>
-      <c r="E54" s="114" t="n"/>
-      <c r="F54" s="114" t="n"/>
-      <c r="G54" s="117" t="n"/>
+      <c r="B54" s="111" t="n"/>
+      <c r="C54" s="111" t="n"/>
+      <c r="D54" s="111" t="n"/>
+      <c r="E54" s="111" t="n"/>
+      <c r="F54" s="111" t="n"/>
+      <c r="G54" s="114" t="n"/>
       <c r="H54" s="2" t="n"/>
       <c r="I54" s="2" t="n"/>
       <c r="J54" s="1" t="n"/>
@@ -2223,12 +2218,12 @@
           <t>COPIA REGISTRO DE IMPORTACIÓN (SOLO IMPORTADOS)</t>
         </is>
       </c>
-      <c r="B55" s="114" t="n"/>
-      <c r="C55" s="114" t="n"/>
-      <c r="D55" s="114" t="n"/>
-      <c r="E55" s="114" t="n"/>
-      <c r="F55" s="114" t="n"/>
-      <c r="G55" s="117" t="n"/>
+      <c r="B55" s="111" t="n"/>
+      <c r="C55" s="111" t="n"/>
+      <c r="D55" s="111" t="n"/>
+      <c r="E55" s="111" t="n"/>
+      <c r="F55" s="111" t="n"/>
+      <c r="G55" s="114" t="n"/>
       <c r="H55" s="2" t="n"/>
       <c r="I55" s="2" t="n"/>
       <c r="J55" s="1" t="n"/>
@@ -2239,12 +2234,12 @@
           <t>COPIA FACTURA</t>
         </is>
       </c>
-      <c r="B56" s="114" t="n"/>
-      <c r="C56" s="114" t="n"/>
-      <c r="D56" s="114" t="n"/>
-      <c r="E56" s="114" t="n"/>
-      <c r="F56" s="114" t="n"/>
-      <c r="G56" s="117" t="n"/>
+      <c r="B56" s="111" t="n"/>
+      <c r="C56" s="111" t="n"/>
+      <c r="D56" s="111" t="n"/>
+      <c r="E56" s="111" t="n"/>
+      <c r="F56" s="111" t="n"/>
+      <c r="G56" s="114" t="n"/>
       <c r="H56" s="2" t="n"/>
       <c r="I56" s="2" t="n"/>
       <c r="J56" s="1" t="n"/>
@@ -2255,12 +2250,12 @@
           <t>COPIA DE INGRESO AL ALMÁCEN</t>
         </is>
       </c>
-      <c r="B57" s="114" t="n"/>
-      <c r="C57" s="114" t="n"/>
-      <c r="D57" s="114" t="n"/>
-      <c r="E57" s="114" t="n"/>
-      <c r="F57" s="114" t="n"/>
-      <c r="G57" s="117" t="n"/>
+      <c r="B57" s="111" t="n"/>
+      <c r="C57" s="111" t="n"/>
+      <c r="D57" s="111" t="n"/>
+      <c r="E57" s="111" t="n"/>
+      <c r="F57" s="111" t="n"/>
+      <c r="G57" s="114" t="n"/>
       <c r="H57" s="2" t="n"/>
       <c r="I57" s="2" t="n"/>
       <c r="J57" s="1" t="n"/>
@@ -2271,12 +2266,12 @@
           <t>COPIA DE ACTA DE RECIBO A SATISFACCIÓN</t>
         </is>
       </c>
-      <c r="B58" s="114" t="n"/>
-      <c r="C58" s="114" t="n"/>
-      <c r="D58" s="114" t="n"/>
-      <c r="E58" s="114" t="n"/>
-      <c r="F58" s="114" t="n"/>
-      <c r="G58" s="117" t="n"/>
+      <c r="B58" s="111" t="n"/>
+      <c r="C58" s="111" t="n"/>
+      <c r="D58" s="111" t="n"/>
+      <c r="E58" s="111" t="n"/>
+      <c r="F58" s="111" t="n"/>
+      <c r="G58" s="114" t="n"/>
       <c r="H58" s="2" t="n"/>
       <c r="I58" s="2" t="n"/>
       <c r="J58" s="1" t="n"/>
@@ -2287,12 +2282,12 @@
           <t>GUÍA RAPIDA DE OPERACIÓN</t>
         </is>
       </c>
-      <c r="B59" s="114" t="n"/>
-      <c r="C59" s="114" t="n"/>
-      <c r="D59" s="114" t="n"/>
-      <c r="E59" s="114" t="n"/>
-      <c r="F59" s="114" t="n"/>
-      <c r="G59" s="117" t="n"/>
+      <c r="B59" s="111" t="n"/>
+      <c r="C59" s="111" t="n"/>
+      <c r="D59" s="111" t="n"/>
+      <c r="E59" s="111" t="n"/>
+      <c r="F59" s="111" t="n"/>
+      <c r="G59" s="114" t="n"/>
       <c r="H59" s="2" t="n"/>
       <c r="I59" s="2" t="n"/>
       <c r="J59" s="1" t="n"/>
@@ -2303,12 +2298,12 @@
           <t>RECOMENDACIÓN DEL FABRICANTE PARA USO DE ACCESORIOS Y CONSUMIBLES</t>
         </is>
       </c>
-      <c r="B60" s="114" t="n"/>
-      <c r="C60" s="114" t="n"/>
-      <c r="D60" s="114" t="n"/>
-      <c r="E60" s="114" t="n"/>
-      <c r="F60" s="114" t="n"/>
-      <c r="G60" s="117" t="n"/>
+      <c r="B60" s="111" t="n"/>
+      <c r="C60" s="111" t="n"/>
+      <c r="D60" s="111" t="n"/>
+      <c r="E60" s="111" t="n"/>
+      <c r="F60" s="111" t="n"/>
+      <c r="G60" s="114" t="n"/>
       <c r="H60" s="2" t="n"/>
       <c r="I60" s="2" t="n"/>
       <c r="J60" s="1" t="n"/>
@@ -2319,12 +2314,12 @@
           <t>RECOMENDACIÓN DEL FABRICANTE PARA ASEGURAMIENTO METROLÓGICO</t>
         </is>
       </c>
-      <c r="B61" s="114" t="n"/>
-      <c r="C61" s="114" t="n"/>
-      <c r="D61" s="114" t="n"/>
-      <c r="E61" s="114" t="n"/>
-      <c r="F61" s="114" t="n"/>
-      <c r="G61" s="117" t="n"/>
+      <c r="B61" s="111" t="n"/>
+      <c r="C61" s="111" t="n"/>
+      <c r="D61" s="111" t="n"/>
+      <c r="E61" s="111" t="n"/>
+      <c r="F61" s="111" t="n"/>
+      <c r="G61" s="114" t="n"/>
       <c r="H61" s="1" t="n"/>
       <c r="I61" s="2" t="n"/>
       <c r="J61" s="1" t="n"/>
@@ -2335,12 +2330,12 @@
           <t>ESTIMATIVO DE COSTO DE ACCESORIOS Y CONSUMIBLES</t>
         </is>
       </c>
-      <c r="B62" s="114" t="n"/>
-      <c r="C62" s="114" t="n"/>
-      <c r="D62" s="114" t="n"/>
-      <c r="E62" s="114" t="n"/>
-      <c r="F62" s="114" t="n"/>
-      <c r="G62" s="117" t="n"/>
+      <c r="B62" s="111" t="n"/>
+      <c r="C62" s="111" t="n"/>
+      <c r="D62" s="111" t="n"/>
+      <c r="E62" s="111" t="n"/>
+      <c r="F62" s="111" t="n"/>
+      <c r="G62" s="114" t="n"/>
       <c r="H62" s="1" t="n"/>
       <c r="I62" s="2" t="n"/>
       <c r="J62" s="1" t="n"/>
@@ -2351,12 +2346,12 @@
           <t xml:space="preserve">RECOMENDACIONES DE LIMPIEZA Y DESINFECCIÓN </t>
         </is>
       </c>
-      <c r="B63" s="114" t="n"/>
-      <c r="C63" s="114" t="n"/>
-      <c r="D63" s="114" t="n"/>
-      <c r="E63" s="114" t="n"/>
-      <c r="F63" s="114" t="n"/>
-      <c r="G63" s="117" t="n"/>
+      <c r="B63" s="111" t="n"/>
+      <c r="C63" s="111" t="n"/>
+      <c r="D63" s="111" t="n"/>
+      <c r="E63" s="111" t="n"/>
+      <c r="F63" s="111" t="n"/>
+      <c r="G63" s="114" t="n"/>
       <c r="H63" s="1" t="n"/>
       <c r="I63" s="2" t="n"/>
       <c r="J63" s="1" t="n"/>
@@ -2367,18 +2362,18 @@
           <t>REGISTRO DE CAPACITACIÓN</t>
         </is>
       </c>
-      <c r="B64" s="114" t="n"/>
-      <c r="C64" s="114" t="n"/>
-      <c r="D64" s="114" t="n"/>
-      <c r="E64" s="114" t="n"/>
-      <c r="F64" s="114" t="n"/>
-      <c r="G64" s="117" t="n"/>
+      <c r="B64" s="111" t="n"/>
+      <c r="C64" s="111" t="n"/>
+      <c r="D64" s="111" t="n"/>
+      <c r="E64" s="111" t="n"/>
+      <c r="F64" s="111" t="n"/>
+      <c r="G64" s="114" t="n"/>
       <c r="H64" s="1" t="n"/>
       <c r="I64" s="2" t="n"/>
       <c r="J64" s="1" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="117">
+  <mergeCells count="121">
     <mergeCell ref="A15:B15"/>
     <mergeCell ref="C15:D15"/>
     <mergeCell ref="A53:G53"/>
@@ -2398,18 +2393,19 @@
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="I20:J20"/>
     <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="H31:J31"/>
     <mergeCell ref="H5:J11"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="H31:J31"/>
     <mergeCell ref="C28:D28"/>
     <mergeCell ref="H23:I23"/>
     <mergeCell ref="A33:D33"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="E20:G20"/>
-    <mergeCell ref="E28:G28"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A30:B30"/>
     <mergeCell ref="A32:J32"/>
+    <mergeCell ref="E28:G28"/>
     <mergeCell ref="C30:D30"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="C14:D14"/>
@@ -2417,22 +2413,22 @@
     <mergeCell ref="E30:G30"/>
     <mergeCell ref="A63:G63"/>
     <mergeCell ref="H25:I25"/>
+    <mergeCell ref="A40:J40"/>
     <mergeCell ref="E36:J36"/>
-    <mergeCell ref="A40:J40"/>
     <mergeCell ref="H27:J27"/>
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="H33:J33"/>
     <mergeCell ref="I43:J43"/>
     <mergeCell ref="E37:J37"/>
     <mergeCell ref="E12:J12"/>
+    <mergeCell ref="D49:J49"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="D49:J49"/>
+    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E33:G33"/>
     <mergeCell ref="E25:F25"/>
+    <mergeCell ref="A55:G55"/>
     <mergeCell ref="A26:D26"/>
     <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A55:G55"/>
     <mergeCell ref="E17:G17"/>
     <mergeCell ref="C18:D18"/>
     <mergeCell ref="A57:G57"/>
@@ -2446,30 +2442,33 @@
     <mergeCell ref="C20:D20"/>
     <mergeCell ref="A58:G58"/>
     <mergeCell ref="C29:D29"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="C10:G10"/>
+    <mergeCell ref="E13:F13"/>
     <mergeCell ref="A60:G60"/>
     <mergeCell ref="C31:D31"/>
     <mergeCell ref="C9:G9"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="E29:G29"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="C23:D23"/>
     <mergeCell ref="A41:J41"/>
+    <mergeCell ref="G13:J13"/>
     <mergeCell ref="A37:D37"/>
     <mergeCell ref="I51:J51"/>
     <mergeCell ref="E14:G14"/>
     <mergeCell ref="A43:B43"/>
     <mergeCell ref="A12:D12"/>
+    <mergeCell ref="H34:J34"/>
     <mergeCell ref="I50:J50"/>
     <mergeCell ref="E43:F43"/>
+    <mergeCell ref="G43:H43"/>
     <mergeCell ref="A24:B24"/>
-    <mergeCell ref="G43:H43"/>
     <mergeCell ref="C24:D24"/>
+    <mergeCell ref="E24:F24"/>
     <mergeCell ref="C6:G6"/>
-    <mergeCell ref="E24:F24"/>
     <mergeCell ref="A38:D38"/>
     <mergeCell ref="A35:J35"/>
     <mergeCell ref="A6:B6"/>
@@ -2483,8 +2482,8 @@
     <mergeCell ref="A64:G64"/>
     <mergeCell ref="E26:J26"/>
     <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E2:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="E2:H3"/>
     <mergeCell ref="A61:G61"/>
     <mergeCell ref="H14:J14"/>
     <mergeCell ref="A54:G54"/>
@@ -2495,7 +2494,7 @@
     <mergeCell ref="H24:I24"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="E29:G29"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" scale="85"/>

</xml_diff>